<commit_message>
fix some dir path
Former-commit-id: ea16949337e76c20c7af030cf9913f2bf091d922 [formerly 5f51ef21c454edb486ae5d36c8ff5acbdd78dad3] [formerly aaec2c815fe880c6ba159240d4f16ee0aa29c1a8 [formerly 8fef08e317033e6da0a75ba385c90868646b45fa]]
Former-commit-id: 3728b8c0fe3345224254063518fc3a40ba8edd11 [formerly 0a9b58cb1e38bc2e5617575a07c54e4469a8beec]
Former-commit-id: e4cfbc552b8f37723ea003d2dc26b599ad2abdd2
</commit_message>
<xml_diff>
--- a/Bin/Server/resource/Excel/Scene.xlsx
+++ b/Bin/Server/resource/Excel/Scene.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cpp\ArkGameFrame\Bin\Server\DataConfig\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARK\Bin\Server\resource\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28695" windowHeight="13050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28695" windowHeight="13050"/>
   </bookViews>
   <sheets>
     <sheet name="DataNode" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="Scene" type="4" refreshedVersion="2" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="Scene" type="4" refreshedVersion="2" background="1" saveData="1">
     <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Ini\NPC\Scene.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
@@ -229,22 +229,12 @@
     <t>34.10933,1.165174,11.49214</t>
   </si>
   <si>
-    <t>../../DataConfig/Ini/Scene/1.xml</t>
+    <t>../resource/Ini/Scene/1.xml</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <r>
-      <t>../../</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>DataConfig</t>
+      <t>../resource</t>
     </r>
     <r>
       <rPr>
@@ -259,17 +249,7 @@
   </si>
   <si>
     <r>
-      <t>../../</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>DataConfig</t>
+      <t>../resource</t>
     </r>
     <r>
       <rPr>
@@ -284,17 +264,7 @@
   </si>
   <si>
     <r>
-      <t>../../</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>DataConfig</t>
+      <t>../resource</t>
     </r>
     <r>
       <rPr>
@@ -309,17 +279,7 @@
   </si>
   <si>
     <r>
-      <t>../../</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>DataConfig</t>
+      <t>../resource</t>
     </r>
     <r>
       <rPr>
@@ -334,17 +294,7 @@
   </si>
   <si>
     <r>
-      <t>../../</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>DataConfig</t>
+      <t>../resource</t>
     </r>
     <r>
       <rPr>
@@ -361,7 +311,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -930,11 +880,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1646,13 +1596,13 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:I7 J7:P7" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:I7 J7:P7">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7"/>
   </dataValidations>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>